<commit_message>
Atualização do exemplo de dados
Atualização do exemplo de dados, para incluir suporte à locais
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\VALENware\VALENtiny\User version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E275AD-6EDA-4BB1-9C17-62A27BF8B5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331FD19B-8A29-484E-944C-E90EA2172FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13749" xr2:uid="{3956E45A-4E70-4CE3-A5B7-50E9F49972BA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>4X31R64405</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>4XD1P83425</t>
+  </si>
+  <si>
+    <t>ZC05</t>
+  </si>
+  <si>
+    <t>SI001</t>
+  </si>
+  <si>
+    <t>ZW06</t>
+  </si>
+  <si>
+    <t>ZC04</t>
+  </si>
+  <si>
+    <t>ZAGNG0301B</t>
   </si>
 </sst>
 </file>
@@ -438,16 +453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D67E4E-5C27-4C36-A3AD-A33C877510EE}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>5272601306</v>
       </c>
@@ -457,8 +473,11 @@
       <c r="C1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5272593676</v>
       </c>
@@ -469,7 +488,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5272594026</v>
       </c>
@@ -480,7 +499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5272594026</v>
       </c>
@@ -491,7 +510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5272594026</v>
       </c>
@@ -502,7 +521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5272595673</v>
       </c>
@@ -512,8 +531,11 @@
       <c r="C6">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5272595667</v>
       </c>
@@ -524,7 +546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5272595667</v>
       </c>
@@ -535,7 +557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5272595667</v>
       </c>
@@ -546,7 +568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5272595667</v>
       </c>
@@ -557,7 +579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5272595667</v>
       </c>
@@ -568,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5272595673</v>
       </c>
@@ -578,8 +600,11 @@
       <c r="C12">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5272595673</v>
       </c>
@@ -589,8 +614,11 @@
       <c r="C13">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5272595673</v>
       </c>
@@ -600,8 +628,11 @@
       <c r="C14">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5272595673</v>
       </c>
@@ -611,8 +642,12 @@
       <c r="C15">
         <v>38</v>
       </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualiza data.xlsx após backup
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -451,187 +451,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D67E4E-5C27-4C36-A3AD-A33C877510EE}">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>5272964724</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5272964724</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5272964724</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5272964724</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5272964724</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>179</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5272964724</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>179</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5272974618</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5272970458</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>91</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5272973084</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>112</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5272973072</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5272973070</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5272973068</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
+<ns0:worksheet xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ns1="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns2="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:ns3="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:ns4="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ns1:Ignorable="x14ac xr xr2 xr3" ns2:uid="{A5D67E4E-5C27-4C36-A3AD-A33C877510EE}">
+  <ns0:dimension ref="A1:D11"/>
+  <ns0:sheetViews>
+    <ns0:sheetView tabSelected="1" workbookViewId="0"/>
+  </ns0:sheetViews>
+  <ns0:sheetFormatPr defaultRowHeight="15" ns3:dyDescent="0.25"/>
+  <ns0:cols>
+    <ns0:col min="1" max="2" width="12.7109375" customWidth="1"/>
+    <ns0:col min="4" max="4" width="12.7109375" customWidth="1"/>
+  </ns0:cols>
+  <ns0:sheetData>
+    <ns0:row r="1" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A1">
+        <ns0:v>5272964724</ns0:v>
+      </ns0:c>
+      <ns0:c r="B1" t="s">
+        <ns0:v>6</ns0:v>
+      </ns0:c>
+      <ns0:c r="C1">
+        <ns0:v>32</ns0:v>
+      </ns0:c>
+      <ns0:c r="D1" t="s">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="2" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A2">
+        <ns0:v>5272964724</ns0:v>
+      </ns0:c>
+      <ns0:c r="B2" t="s">
+        <ns0:v>7</ns0:v>
+      </ns0:c>
+      <ns0:c r="C2">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="D2" t="s">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="3" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A3">
+        <ns0:v>5272964724</ns0:v>
+      </ns0:c>
+      <ns0:c r="B3" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="C3">
+        <ns0:v>78</ns0:v>
+      </ns0:c>
+      <ns0:c r="D3" t="s">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="4" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A4">
+        <ns0:v>5272964724</ns0:v>
+      </ns0:c>
+      <ns0:c r="B4" t="s">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="C4">
+        <ns0:v>1</ns0:v>
+      </ns0:c>
+      <ns0:c r="D4" t="s">
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="5" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A5">
+        <ns0:v>5272964724</ns0:v>
+      </ns0:c>
+      <ns0:c r="B5" t="s">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="C5">
+        <ns0:v>179</ns0:v>
+      </ns0:c>
+      <ns0:c r="D5" t="s">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="6" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A6">
+        <ns0:v>5272964724</ns0:v>
+      </ns0:c>
+      <ns0:c r="B6" t="s">
+        <ns0:v>11</ns0:v>
+      </ns0:c>
+      <ns0:c r="C6">
+        <ns0:v>179</ns0:v>
+      </ns0:c>
+      <ns0:c r="D6" t="s">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="7" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A7">
+        <ns0:v>5272974618</ns0:v>
+      </ns0:c>
+      <ns0:c r="B7" t="s">
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="C7">
+        <ns0:v>1</ns0:v>
+      </ns0:c>
+      <ns0:c r="D7" t="s">
+        <ns0:v>3</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="8" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A8">
+        <ns0:v>5272970458</ns0:v>
+      </ns0:c>
+      <ns0:c r="B8" t="s">
+        <ns0:v>12</ns0:v>
+      </ns0:c>
+      <ns0:c r="C8">
+        <ns0:v>91</ns0:v>
+      </ns0:c>
+      <ns0:c r="D8" t="s">
+        <ns0:v>3</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="9" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A9">
+        <ns0:v>5272973084</ns0:v>
+      </ns0:c>
+      <ns0:c r="B9" t="s">
+        <ns0:v>4</ns0:v>
+      </ns0:c>
+      <ns0:c r="C9">
+        <ns0:v>112</ns0:v>
+      </ns0:c>
+      <ns0:c r="D9" t="s">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="11" spans="1:4" ns3:dyDescent="0.25">
+      <ns0:c r="A11">
+        <ns0:v>5272973070</ns0:v>
+      </ns0:c>
+      <ns0:c r="B11" t="s">
+        <ns0:v>14</ns0:v>
+      </ns0:c>
+      <ns0:c r="C11">
+        <ns0:v>2</ns0:v>
+      </ns0:c>
+      <ns0:c r="D11" t="s">
+        <ns0:v>2</ns0:v>
+      </ns0:c>
+    </ns0:row>
+  </ns0:sheetData>
+  <ns0:pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ns0:pageSetup paperSize="9" orientation="portrait" ns4:id="rId1"/>
+</ns0:worksheet>
 </file>
</xml_diff>